<commit_message>
Update Dormant Sites Reclamation Program - Evidence of Cost.xlsx
</commit_message>
<xml_diff>
--- a/services/dsrp-web/src/assets/downloads/Dormant Sites Reclamation Program - Evidence of Cost.xlsx
+++ b/services/dsrp-web/src/assets/downloads/Dormant Sites Reclamation Program - Evidence of Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\source\repos\dormant-site-reclamation-program\services\dsrp-web\src\assets\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\SFP.IDIR.BCGOV\U161\RESTEVEN$\Profile\Desktop\Dormant Sites\IT Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCB3522-C0BC-4E54-A01E-B577B3CD9009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31F1665-8B29-47A7-97B7-E157A74D1DDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="3840" windowWidth="28780" windowHeight="15450" xr2:uid="{CA0C0557-EF29-410C-A643-F0A2B823516D}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="21262" windowHeight="12772" xr2:uid="{CA0C0557-EF29-410C-A643-F0A2B823516D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Invoice Number</t>
   </si>
@@ -39,23 +45,29 @@
     <t>Vendor Name</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>$ amount</t>
-  </si>
-  <si>
-    <t>Free text</t>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Qualification (e.g. CEO, CFO)</t>
   </si>
   <si>
     <t>Invoice Date (yyyy-mm-dd)</t>
+  </si>
+  <si>
+    <t>I certify that this is a true copy of the document produced to me on [date]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,16 +83,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -88,15 +120,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,54 +474,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEE9D7E-A780-4A58-B331-B98DFDEE61D2}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1"/>
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5"/>
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>